<commit_message>
Read Data From spreadsheet and save updated data // update system to lock login failed attempts
</commit_message>
<xml_diff>
--- a/BankProject/BankProject/writeExcelOutput.xlsx
+++ b/BankProject/BankProject/writeExcelOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>USERINDEX</t>
   </si>
@@ -25,22 +25,16 @@
     <t>USERPASS</t>
   </si>
   <si>
-    <t>ACCOUNT TYPE</t>
-  </si>
-  <si>
-    <t>BALANCE</t>
+    <t>SAVINGS</t>
+  </si>
+  <si>
+    <t>SALARY</t>
   </si>
   <si>
     <t>maria</t>
   </si>
   <si>
     <t>1234</t>
-  </si>
-  <si>
-    <t>Savings</t>
-  </si>
-  <si>
-    <t>Salary</t>
   </si>
   <si>
     <t>pedro</t>
@@ -170,144 +164,75 @@
       <c r="A2" s="2">
         <v>0</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="3">
+        <v>300</v>
+      </c>
     </row>
     <row r="3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>100</v>
       </c>
     </row>
     <row r="4">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D4" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="5">
-      <c r="D5" s="3" t="s">
-        <v>7</v>
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
       <c r="E6" s="3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="E8" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="D12" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="E13" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="D17" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="E18" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="C21" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="D22" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="E23" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="C26" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="D27" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="E28" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="D29" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="E30" s="3">
         <v>0</v>
       </c>
     </row>
@@ -327,77 +252,77 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to save 2-digits value
</commit_message>
<xml_diff>
--- a/BankProject/BankProject/writeExcelOutput.xlsx
+++ b/BankProject/BankProject/writeExcelOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>USERINDEX</t>
   </si>
@@ -37,13 +37,28 @@
     <t>1234</t>
   </si>
   <si>
+    <t>10 394,78 kr</t>
+  </si>
+  <si>
+    <t>330,32 kr</t>
+  </si>
+  <si>
     <t>pedro</t>
   </si>
   <si>
+    <t>110,22 kr</t>
+  </si>
+  <si>
     <t>kalle</t>
   </si>
   <si>
+    <t>100,00 kr</t>
+  </si>
+  <si>
     <t>johan</t>
+  </si>
+  <si>
+    <t>0,00 kr</t>
   </si>
   <si>
     <t>matias</t>
@@ -170,11 +185,11 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3">
-        <v>1000</v>
-      </c>
-      <c r="E2" s="3">
-        <v>300</v>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -182,13 +197,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3">
-        <v>100</v>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -196,13 +211,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3">
-        <v>100</v>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -210,13 +225,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3">
-        <v>0</v>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -224,16 +239,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -252,77 +267,77 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 2-digits values database
</commit_message>
<xml_diff>
--- a/BankProject/BankProject/writeExcelOutput.xlsx
+++ b/BankProject/BankProject/writeExcelOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>USERINDEX</t>
   </si>
@@ -37,28 +37,13 @@
     <t>1234</t>
   </si>
   <si>
-    <t>10 394,78 kr</t>
-  </si>
-  <si>
-    <t>330,32 kr</t>
-  </si>
-  <si>
     <t>pedro</t>
   </si>
   <si>
-    <t>110,22 kr</t>
-  </si>
-  <si>
     <t>kalle</t>
   </si>
   <si>
-    <t>100,00 kr</t>
-  </si>
-  <si>
     <t>johan</t>
-  </si>
-  <si>
-    <t>0,00 kr</t>
   </si>
   <si>
     <t>matias</t>
@@ -185,11 +170,11 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
+      <c r="D2" s="3">
+        <v>10.35</v>
+      </c>
+      <c r="E2" s="3">
+        <v>10.1</v>
       </c>
     </row>
     <row r="3">
@@ -197,13 +182,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
+      <c r="D3" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -211,13 +196,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
+      <c r="D4" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -225,13 +210,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
+      <c r="E5" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -239,16 +224,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -267,77 +252,77 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>